<commit_message>
Fig6 E heatmap added
</commit_message>
<xml_diff>
--- a/Colouring_tab.xlsx
+++ b/Colouring_tab.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="94">
   <si>
     <t xml:space="preserve">Numbers</t>
   </si>
@@ -61,16 +61,16 @@
     <t xml:space="preserve">Fig6D_name</t>
   </si>
   <si>
-    <t xml:space="preserve">Fig6E_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig6E_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig6Eaxis_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig6Eaxis_name</t>
+    <t xml:space="preserve">Fig6Eaci_axis_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig6Eaci_axis_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig6Ephage_axis_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig6Ephage_axis_name</t>
   </si>
   <si>
     <t xml:space="preserve">Fig6F_number</t>
@@ -79,40 +79,52 @@
     <t xml:space="preserve">Fig6F_name</t>
   </si>
   <si>
-    <t xml:space="preserve">Fig7Aaci_axis_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7Aaci_axis_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7Aphage_axis_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7Aphage_axis_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7B_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7B_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7Caci_axis_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7Caci_axis_name</t>
+    <t xml:space="preserve">Fig6Faxis_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig6Faxis_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig6G_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig6G_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7A1st_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7A1st_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7A2nd_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7A2nd_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7A3rd_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7A3rd_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7Baci_axis_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7Baci_axis_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7C_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7C_name</t>
   </si>
   <si>
     <t xml:space="preserve">Fig7D_number</t>
   </si>
   <si>
     <t xml:space="preserve">Fig7D_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7E_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7E_name</t>
   </si>
   <si>
     <t xml:space="preserve">gray</t>
@@ -463,7 +475,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -481,6 +493,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -649,17 +665,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF14"/>
+  <dimension ref="A1:AJ14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="AC2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AC1" activeCellId="0" sqref="AC1"/>
+      <selection pane="topRight" activeCell="O1" activeCellId="0" sqref="O1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD2" activeCellId="0" sqref="AD2"/>
+      <selection pane="bottomRight" activeCell="P4" activeCellId="0" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.7"/>
@@ -674,16 +690,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="15.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="18.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="13.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="11.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="15.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="18.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="11.97"/>
@@ -692,10 +708,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="15.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="11.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="15.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="11.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="15.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="11.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="15.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="6" customFormat="true" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -738,22 +758,22 @@
       <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="4" t="s">
@@ -768,19 +788,19 @@
       <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="5" t="s">
         <v>28</v>
       </c>
       <c r="AD1" s="3" t="s">
@@ -789,173 +809,201 @@
       <c r="AE1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2"/>
+      <c r="AF1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="2"/>
     </row>
-    <row r="2" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="n">
+    <row r="2" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="8" t="n">
+      <c r="B2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="6" t="n">
+      <c r="G2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="8" t="n">
+      <c r="I2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6" t="n">
+      <c r="K2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="Q2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="R2" s="6" t="n">
+      <c r="O2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="8" t="n">
+      <c r="U2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="X2" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB2" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH2" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="U2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="Y2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD2" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF2" s="6"/>
+      <c r="AI2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="12"/>
+        <v>43</v>
+      </c>
+      <c r="D3" s="13"/>
       <c r="E3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="13" t="n">
+        <v>44</v>
+      </c>
+      <c r="F3" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>40</v>
+      <c r="G3" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="9"/>
+        <v>44</v>
+      </c>
+      <c r="J3" s="14"/>
+      <c r="K3" s="10"/>
       <c r="L3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N3" s="13" t="n">
+        <v>45</v>
+      </c>
+      <c r="N3" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="P3" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R3" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P3" s="1" t="n">
+      <c r="S3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="Q3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="R3" s="1" t="n">
+      <c r="U3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="V3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X3" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z3" s="15"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="15"/>
+      <c r="AC3" s="11"/>
+      <c r="AD3" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T3" s="13" t="n">
+      <c r="AE3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF3" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH3" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="U3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="V3" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="X3" s="13" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z3" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA3" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB3" s="13" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD3" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE3" s="9" t="s">
-        <v>45</v>
+      <c r="AI3" s="10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -963,502 +1011,542 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="15"/>
+        <v>51</v>
+      </c>
+      <c r="D4" s="16"/>
       <c r="E4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="13" t="n">
+        <v>52</v>
+      </c>
+      <c r="F4" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>48</v>
+      <c r="G4" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="9"/>
+        <v>52</v>
+      </c>
+      <c r="J4" s="14"/>
+      <c r="K4" s="10"/>
       <c r="L4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N4" s="13" t="n">
+        <v>53</v>
+      </c>
+      <c r="N4" s="14"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q4" s="9"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="14" t="n">
-        <v>2</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10"/>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="13"/>
-      <c r="AE4" s="9"/>
+      <c r="S4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U4" s="10"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="15"/>
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="11"/>
+      <c r="AF4" s="14"/>
+      <c r="AG4" s="10"/>
+      <c r="AH4" s="14"/>
+      <c r="AI4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="16"/>
+        <v>55</v>
+      </c>
+      <c r="D5" s="17"/>
       <c r="E5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="9"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="9"/>
-      <c r="N5" s="13" t="n">
+        <v>56</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="10"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="10"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R5" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q5" s="9"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="14" t="n">
-        <v>3</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="10"/>
-      <c r="AA5" s="10"/>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="9"/>
-      <c r="AD5" s="13"/>
-      <c r="AE5" s="9"/>
+      <c r="S5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U5" s="10"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="11"/>
+      <c r="AF5" s="14"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="14"/>
+      <c r="AI5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="17"/>
+        <v>58</v>
+      </c>
+      <c r="D6" s="18"/>
       <c r="E6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="9"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="9"/>
-      <c r="N6" s="13" t="n">
+        <v>59</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="10"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="10"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="R6" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q6" s="9"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="14" t="n">
-        <v>4</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="18"/>
-      <c r="Z6" s="14"/>
-      <c r="AA6" s="14"/>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="18"/>
-      <c r="AD6" s="13"/>
-      <c r="AE6" s="18"/>
+      <c r="S6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="U6" s="10"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="15"/>
+      <c r="AF6" s="14"/>
+      <c r="AG6" s="19"/>
+      <c r="AH6" s="14"/>
+      <c r="AI6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="19"/>
+        <v>61</v>
+      </c>
+      <c r="D7" s="20"/>
       <c r="E7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="13" t="n">
+        <v>62</v>
+      </c>
+      <c r="F7" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>58</v>
+      <c r="G7" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>4</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="J7" s="14"/>
+      <c r="K7" s="10"/>
       <c r="L7" s="1" t="n">
         <v>3</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N7" s="13"/>
-      <c r="P7" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="N7" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="Q7" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="R7" s="1" t="n">
+      <c r="O7" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="14"/>
+      <c r="T7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="S7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="T7" s="13" t="n">
+      <c r="U7" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="V7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="U7" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="V7" s="10"/>
-      <c r="W7" s="10"/>
-      <c r="X7" s="13" t="n">
+      <c r="AA7" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB7" s="15"/>
+      <c r="AC7" s="15"/>
+      <c r="AD7" s="14"/>
+      <c r="AE7" s="15"/>
+      <c r="AF7" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="Y7" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z7" s="14"/>
-      <c r="AA7" s="14"/>
-      <c r="AB7" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="AC7" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD7" s="13"/>
-      <c r="AE7" s="18"/>
+      <c r="AG7" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH7" s="14"/>
+      <c r="AI7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="20"/>
+        <v>68</v>
+      </c>
+      <c r="D8" s="21"/>
       <c r="E8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="9"/>
+        <v>69</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="10"/>
       <c r="H8" s="1" t="n">
         <v>5</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="9"/>
-      <c r="N8" s="13"/>
-      <c r="Q8" s="9"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="18"/>
-      <c r="Z8" s="14"/>
-      <c r="AA8" s="14"/>
-      <c r="AB8" s="13"/>
-      <c r="AC8" s="18"/>
-      <c r="AD8" s="13"/>
-      <c r="AE8" s="18"/>
+        <v>69</v>
+      </c>
+      <c r="J8" s="14"/>
+      <c r="K8" s="10"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="14"/>
+      <c r="U8" s="10"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="15"/>
+      <c r="AC8" s="15"/>
+      <c r="AD8" s="14"/>
+      <c r="AE8" s="15"/>
+      <c r="AF8" s="14"/>
+      <c r="AG8" s="19"/>
+      <c r="AH8" s="14"/>
+      <c r="AI8" s="19"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="21"/>
+        <v>71</v>
+      </c>
+      <c r="D9" s="22"/>
       <c r="E9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="9"/>
+        <v>72</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="10"/>
       <c r="H9" s="1" t="n">
         <v>6</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="9"/>
-      <c r="N9" s="13"/>
-      <c r="Q9" s="9"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="13"/>
-      <c r="Y9" s="18"/>
-      <c r="Z9" s="14"/>
-      <c r="AA9" s="14"/>
-      <c r="AB9" s="13"/>
-      <c r="AC9" s="18"/>
-      <c r="AD9" s="13"/>
-      <c r="AE9" s="18"/>
+        <v>72</v>
+      </c>
+      <c r="J9" s="14"/>
+      <c r="K9" s="10"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="14"/>
+      <c r="U9" s="10"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="15"/>
+      <c r="AB9" s="15"/>
+      <c r="AC9" s="15"/>
+      <c r="AD9" s="14"/>
+      <c r="AE9" s="15"/>
+      <c r="AF9" s="14"/>
+      <c r="AG9" s="19"/>
+      <c r="AH9" s="14"/>
+      <c r="AI9" s="19"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="22"/>
+        <v>74</v>
+      </c>
+      <c r="D10" s="23"/>
       <c r="E10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="9"/>
+        <v>75</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="10"/>
       <c r="H10" s="1" t="n">
         <v>7</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="9"/>
-      <c r="N10" s="13"/>
-      <c r="Q10" s="9"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="18"/>
-      <c r="Z10" s="14"/>
-      <c r="AA10" s="14"/>
-      <c r="AB10" s="13"/>
-      <c r="AC10" s="18"/>
-      <c r="AD10" s="13"/>
-      <c r="AE10" s="18"/>
+        <v>75</v>
+      </c>
+      <c r="J10" s="14"/>
+      <c r="K10" s="10"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="14"/>
+      <c r="U10" s="10"/>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
+      <c r="AA10" s="15"/>
+      <c r="AB10" s="15"/>
+      <c r="AC10" s="15"/>
+      <c r="AD10" s="14"/>
+      <c r="AE10" s="15"/>
+      <c r="AF10" s="14"/>
+      <c r="AG10" s="19"/>
+      <c r="AH10" s="14"/>
+      <c r="AI10" s="19"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="23"/>
+        <v>77</v>
+      </c>
+      <c r="D11" s="24"/>
       <c r="E11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="9"/>
+        <v>78</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="10"/>
       <c r="H11" s="1" t="n">
         <v>8</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="9"/>
+        <v>78</v>
+      </c>
+      <c r="J11" s="14"/>
+      <c r="K11" s="10"/>
       <c r="L11" s="1" t="n">
         <v>4</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N11" s="13"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="T11" s="13"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="10"/>
-      <c r="W11" s="10"/>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="18"/>
-      <c r="Z11" s="14"/>
-      <c r="AA11" s="14"/>
-      <c r="AB11" s="13"/>
-      <c r="AC11" s="18"/>
-      <c r="AD11" s="13"/>
-      <c r="AE11" s="18"/>
+        <v>79</v>
+      </c>
+      <c r="N11" s="14"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="14"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
+      <c r="AB11" s="15"/>
+      <c r="AC11" s="15"/>
+      <c r="AD11" s="14"/>
+      <c r="AE11" s="15"/>
+      <c r="AF11" s="14"/>
+      <c r="AG11" s="19"/>
+      <c r="AH11" s="14"/>
+      <c r="AI11" s="19"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" s="24"/>
+        <v>82</v>
+      </c>
+      <c r="D12" s="25"/>
       <c r="E12" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="9"/>
+        <v>83</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="10"/>
       <c r="H12" s="1" t="n">
         <v>10</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="9"/>
-      <c r="N12" s="13"/>
-      <c r="Q12" s="9"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="10"/>
-      <c r="W12" s="10"/>
-      <c r="X12" s="13"/>
-      <c r="Y12" s="18"/>
-      <c r="Z12" s="14"/>
-      <c r="AA12" s="14"/>
-      <c r="AB12" s="13"/>
-      <c r="AC12" s="18"/>
-      <c r="AD12" s="13"/>
-      <c r="AE12" s="18"/>
+        <v>83</v>
+      </c>
+      <c r="J12" s="14"/>
+      <c r="K12" s="10"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="14"/>
+      <c r="U12" s="10"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="15"/>
+      <c r="AA12" s="15"/>
+      <c r="AB12" s="15"/>
+      <c r="AC12" s="15"/>
+      <c r="AD12" s="14"/>
+      <c r="AE12" s="15"/>
+      <c r="AF12" s="14"/>
+      <c r="AG12" s="19"/>
+      <c r="AH12" s="14"/>
+      <c r="AI12" s="19"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D13" s="25"/>
+        <v>85</v>
+      </c>
+      <c r="D13" s="26"/>
       <c r="E13" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="9"/>
+        <v>86</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="10"/>
       <c r="H13" s="1" t="n">
         <v>9</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J13" s="13" t="n">
+        <v>86</v>
+      </c>
+      <c r="J13" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="K13" s="9" t="s">
-        <v>82</v>
+      <c r="K13" s="10" t="s">
+        <v>86</v>
       </c>
       <c r="L13" s="1" t="n">
         <v>5</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="N13" s="13"/>
-      <c r="P13" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="N13" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="Q13" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="R13" s="1" t="n">
+      <c r="O13" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="14"/>
+      <c r="T13" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="U13" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="V13" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="X13" s="14"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC13" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD13" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE13" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF13" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="S13" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="T13" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="U13" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="V13" s="10"/>
-      <c r="W13" s="10"/>
-      <c r="X13" s="13" t="n">
-        <v>5</v>
-      </c>
-      <c r="Y13" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z13" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA13" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB13" s="13" t="n">
-        <v>5</v>
-      </c>
-      <c r="AC13" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="AD13" s="13" t="n">
+      <c r="AG13" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="AH13" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="AE13" s="9" t="s">
-        <v>87</v>
+      <c r="AI13" s="10" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1466,35 +1554,47 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D14" s="26"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="18"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="18"/>
-      <c r="N14" s="13"/>
-      <c r="Q14" s="18"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="13" t="n">
+        <v>92</v>
+      </c>
+      <c r="D14" s="27"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="19"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="19"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="14"/>
+      <c r="U14" s="19"/>
+      <c r="X14" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="Y14" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z14" s="14"/>
-      <c r="AA14" s="14"/>
-      <c r="AB14" s="13" t="n">
+      <c r="Y14" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z14" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="AC14" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD14" s="13"/>
-      <c r="AE14" s="18"/>
+      <c r="AA14" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB14" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD14" s="14"/>
+      <c r="AE14" s="15"/>
+      <c r="AF14" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG14" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH14" s="14"/>
+      <c r="AI14" s="19"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Fig 7 A script improvement
</commit_message>
<xml_diff>
--- a/Colouring_tab.xlsx
+++ b/Colouring_tab.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="100">
   <si>
     <t xml:space="preserve">Numbers</t>
   </si>
@@ -109,6 +109,12 @@
     <t xml:space="preserve">Fig7A3rd_name</t>
   </si>
   <si>
+    <t xml:space="preserve">Fig7Alegend_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7Alegend_name</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fig7Baci_axis_number</t>
   </si>
   <si>
@@ -169,23 +175,7 @@
     <t xml:space="preserve">H&lt;sup&gt;R&lt;/sup&gt;</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">A110-1 H</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&lt;sup&gt;R&lt;/sup&gt;</t>
-    </r>
+    <t xml:space="preserve">A110-1 H&lt;sup&gt;R&lt;/sup&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">A107-E1</t>
@@ -242,23 +232,7 @@
     <t xml:space="preserve">HS&lt;sup&gt;R&lt;/sup&gt;</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">A110-2 HS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&lt;sup&gt;R&lt;/sup&gt;</t>
-    </r>
+    <t xml:space="preserve">A110-2 HS&lt;sup&gt;R&lt;/sup&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Aci 110 + HS</t>
@@ -333,23 +307,7 @@
     <t xml:space="preserve">HSFPh&lt;sup&gt;R&lt;/sup&gt;</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">A110-G1 HSFPh</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&lt;sup&gt;R&lt;/sup&gt;</t>
-    </r>
+    <t xml:space="preserve">A110-G1 HSFPh&lt;sup&gt;R&lt;/sup&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Aci 110 + HSFPh</t>
@@ -371,7 +329,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -399,11 +357,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="15">
@@ -730,17 +683,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AJ14"/>
+  <dimension ref="A1:AL14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="W1" activeCellId="0" sqref="W1"/>
+      <selection pane="topRight" activeCell="X1" activeCellId="0" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC18" activeCellId="0" sqref="AC18"/>
+      <selection pane="bottomRight" activeCell="AC14" activeCellId="0" sqref="AC14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.7"/>
@@ -772,12 +725,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="11.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="27.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="11.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="15.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="27.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="11.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="15.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="11.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="15.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="11.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="15.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -868,10 +823,10 @@
       <c r="AC1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="5" t="s">
         <v>30</v>
       </c>
       <c r="AF1" s="3" t="s">
@@ -886,39 +841,45 @@
       <c r="AI1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2"/>
+      <c r="AJ1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="2"/>
     </row>
     <row r="2" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F2" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H2" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J2" s="9" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
@@ -926,7 +887,7 @@
         <v>1</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
@@ -936,13 +897,13 @@
         <v>1</v>
       </c>
       <c r="U2" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="V2" s="7" t="n">
         <v>5</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="X2" s="9" t="n">
         <v>2</v>
@@ -962,47 +923,53 @@
       <c r="AC2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="AG2" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="AD2" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="11"/>
       <c r="AH2" s="9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI2" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ2" s="7"/>
+        <v>41</v>
+      </c>
+      <c r="AJ2" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F3" s="14" t="n">
         <v>2</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J3" s="14"/>
       <c r="K3" s="10"/>
@@ -1010,37 +977,37 @@
         <v>1</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="N3" s="14" t="n">
         <v>2</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="P3" s="15" t="n">
         <v>4</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="R3" s="14" t="n">
         <v>1</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="T3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="U3" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="V3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="X3" s="14" t="n">
         <v>3</v>
@@ -1052,23 +1019,29 @@
       <c r="AA3" s="11"/>
       <c r="AB3" s="15"/>
       <c r="AC3" s="11"/>
-      <c r="AD3" s="9" t="n">
-        <v>2</v>
+      <c r="AD3" s="11" t="n">
+        <v>3</v>
       </c>
       <c r="AE3" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF3" s="14" t="n">
+        <v>51</v>
+      </c>
+      <c r="AF3" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH3" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="AG3" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="AH3" s="14" t="n">
-        <v>2</v>
-      </c>
       <c r="AI3" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="AJ3" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK3" s="10" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,26 +1049,26 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F4" s="14" t="n">
         <v>3</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J4" s="14"/>
       <c r="K4" s="10"/>
@@ -1103,7 +1076,7 @@
         <v>2</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N4" s="14"/>
       <c r="O4" s="11"/>
@@ -1111,13 +1084,13 @@
         <v>3</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="R4" s="14" t="n">
         <v>2</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="U4" s="10"/>
       <c r="X4" s="14"/>
@@ -1126,26 +1099,28 @@
       <c r="AA4" s="11"/>
       <c r="AB4" s="15"/>
       <c r="AC4" s="11"/>
-      <c r="AD4" s="9"/>
+      <c r="AD4" s="11"/>
       <c r="AE4" s="11"/>
-      <c r="AF4" s="14"/>
-      <c r="AG4" s="10"/>
+      <c r="AF4" s="9"/>
+      <c r="AG4" s="11"/>
       <c r="AH4" s="14"/>
       <c r="AI4" s="10"/>
+      <c r="AJ4" s="14"/>
+      <c r="AK4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="10"/>
@@ -1158,13 +1133,13 @@
         <v>2</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="R5" s="14" t="n">
         <v>3</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U5" s="10"/>
       <c r="X5" s="14"/>
@@ -1173,26 +1148,28 @@
       <c r="AA5" s="11"/>
       <c r="AB5" s="15"/>
       <c r="AC5" s="11"/>
-      <c r="AD5" s="9"/>
+      <c r="AD5" s="11"/>
       <c r="AE5" s="11"/>
-      <c r="AF5" s="14"/>
-      <c r="AG5" s="10"/>
+      <c r="AF5" s="9"/>
+      <c r="AG5" s="11"/>
       <c r="AH5" s="14"/>
       <c r="AI5" s="10"/>
+      <c r="AJ5" s="14"/>
+      <c r="AK5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="10"/>
@@ -1205,13 +1182,13 @@
         <v>1</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="R6" s="14" t="n">
         <v>4</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="U6" s="10"/>
       <c r="X6" s="14"/>
@@ -1220,38 +1197,40 @@
       <c r="AA6" s="15"/>
       <c r="AB6" s="15"/>
       <c r="AC6" s="15"/>
-      <c r="AD6" s="14"/>
+      <c r="AD6" s="15"/>
       <c r="AE6" s="15"/>
       <c r="AF6" s="14"/>
-      <c r="AG6" s="19"/>
+      <c r="AG6" s="15"/>
       <c r="AH6" s="14"/>
       <c r="AI6" s="19"/>
+      <c r="AJ6" s="14"/>
+      <c r="AK6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F7" s="14" t="n">
         <v>4</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>4</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J7" s="14"/>
       <c r="K7" s="10"/>
@@ -1259,13 +1238,13 @@
         <v>3</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="N7" s="14" t="n">
         <v>3</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -1274,13 +1253,13 @@
         <v>3</v>
       </c>
       <c r="U7" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="V7" s="1" t="n">
         <v>2</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="X7" s="14"/>
       <c r="Y7" s="15"/>
@@ -1292,30 +1271,36 @@
       </c>
       <c r="AB7" s="15"/>
       <c r="AC7" s="15"/>
-      <c r="AD7" s="14"/>
-      <c r="AE7" s="15"/>
-      <c r="AF7" s="14" t="n">
+      <c r="AD7" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="AG7" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="AH7" s="14"/>
-      <c r="AI7" s="19"/>
+      <c r="AE7" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF7" s="14"/>
+      <c r="AG7" s="15"/>
+      <c r="AH7" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI7" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ7" s="14"/>
+      <c r="AK7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="10"/>
@@ -1323,7 +1308,7 @@
         <v>5</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J8" s="14"/>
       <c r="K8" s="10"/>
@@ -1339,26 +1324,28 @@
       <c r="AA8" s="15"/>
       <c r="AB8" s="15"/>
       <c r="AC8" s="15"/>
-      <c r="AD8" s="14"/>
+      <c r="AD8" s="15"/>
       <c r="AE8" s="15"/>
       <c r="AF8" s="14"/>
-      <c r="AG8" s="19"/>
+      <c r="AG8" s="15"/>
       <c r="AH8" s="14"/>
       <c r="AI8" s="19"/>
+      <c r="AJ8" s="14"/>
+      <c r="AK8" s="19"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="10"/>
@@ -1366,7 +1353,7 @@
         <v>6</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J9" s="14"/>
       <c r="K9" s="10"/>
@@ -1382,26 +1369,28 @@
       <c r="AA9" s="15"/>
       <c r="AB9" s="15"/>
       <c r="AC9" s="15"/>
-      <c r="AD9" s="14"/>
+      <c r="AD9" s="15"/>
       <c r="AE9" s="15"/>
       <c r="AF9" s="14"/>
-      <c r="AG9" s="19"/>
+      <c r="AG9" s="15"/>
       <c r="AH9" s="14"/>
       <c r="AI9" s="19"/>
+      <c r="AJ9" s="14"/>
+      <c r="AK9" s="19"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="10"/>
@@ -1409,7 +1398,7 @@
         <v>7</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J10" s="14"/>
       <c r="K10" s="10"/>
@@ -1425,26 +1414,28 @@
       <c r="AA10" s="15"/>
       <c r="AB10" s="15"/>
       <c r="AC10" s="15"/>
-      <c r="AD10" s="14"/>
+      <c r="AD10" s="15"/>
       <c r="AE10" s="15"/>
       <c r="AF10" s="14"/>
-      <c r="AG10" s="19"/>
+      <c r="AG10" s="15"/>
       <c r="AH10" s="14"/>
       <c r="AI10" s="19"/>
+      <c r="AJ10" s="14"/>
+      <c r="AK10" s="19"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="10"/>
@@ -1452,7 +1443,7 @@
         <v>8</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="10"/>
@@ -1460,7 +1451,7 @@
         <v>4</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N11" s="14"/>
       <c r="O11" s="11"/>
@@ -1472,7 +1463,7 @@
         <v>3</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="X11" s="14"/>
       <c r="Y11" s="15"/>
@@ -1480,26 +1471,28 @@
       <c r="AA11" s="15"/>
       <c r="AB11" s="15"/>
       <c r="AC11" s="15"/>
-      <c r="AD11" s="14"/>
+      <c r="AD11" s="15"/>
       <c r="AE11" s="15"/>
       <c r="AF11" s="14"/>
-      <c r="AG11" s="19"/>
+      <c r="AG11" s="15"/>
       <c r="AH11" s="14"/>
       <c r="AI11" s="19"/>
+      <c r="AJ11" s="14"/>
+      <c r="AK11" s="19"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="10"/>
@@ -1507,7 +1500,7 @@
         <v>10</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="J12" s="14"/>
       <c r="K12" s="10"/>
@@ -1523,26 +1516,28 @@
       <c r="AA12" s="15"/>
       <c r="AB12" s="15"/>
       <c r="AC12" s="15"/>
-      <c r="AD12" s="14"/>
+      <c r="AD12" s="15"/>
       <c r="AE12" s="15"/>
       <c r="AF12" s="14"/>
-      <c r="AG12" s="19"/>
+      <c r="AG12" s="15"/>
       <c r="AH12" s="14"/>
       <c r="AI12" s="19"/>
+      <c r="AJ12" s="14"/>
+      <c r="AK12" s="19"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="10"/>
@@ -1550,25 +1545,25 @@
         <v>9</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J13" s="14" t="n">
         <v>2</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L13" s="1" t="n">
         <v>5</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="N13" s="14" t="n">
         <v>4</v>
       </c>
       <c r="O13" s="11" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
@@ -1577,13 +1572,13 @@
         <v>4</v>
       </c>
       <c r="U13" s="10" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="V13" s="1" t="n">
         <v>4</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="X13" s="14"/>
       <c r="Y13" s="11"/>
@@ -1595,23 +1590,29 @@
       <c r="AC13" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="AD13" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE13" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF13" s="14" t="n">
+      <c r="AD13" s="11" t="n">
         <v>5</v>
       </c>
+      <c r="AE13" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF13" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="AG13" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AH13" s="14" t="n">
+        <v>5</v>
+      </c>
+      <c r="AI13" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ13" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="AI13" s="10" t="s">
-        <v>95</v>
+      <c r="AK13" s="10" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1619,7 +1620,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D14" s="27"/>
       <c r="F14" s="14"/>
@@ -1636,30 +1637,36 @@
         <v>1</v>
       </c>
       <c r="Y14" s="15" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="Z14" s="15" t="n">
         <v>1</v>
       </c>
       <c r="AA14" s="15" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="AB14" s="15" t="n">
         <v>1</v>
       </c>
       <c r="AC14" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD14" s="14"/>
-      <c r="AE14" s="15"/>
-      <c r="AF14" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG14" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="AH14" s="14"/>
-      <c r="AI14" s="19"/>
+        <v>99</v>
+      </c>
+      <c r="AD14" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE14" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF14" s="14"/>
+      <c r="AG14" s="15"/>
+      <c r="AH14" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI14" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="AJ14" s="14"/>
+      <c r="AK14" s="19"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Fig 7 A B C legend OK
</commit_message>
<xml_diff>
--- a/Colouring_tab.xlsx
+++ b/Colouring_tab.xlsx
@@ -91,34 +91,16 @@
     <t xml:space="preserve">Fig6G_name</t>
   </si>
   <si>
-    <t xml:space="preserve">Fig7A1st_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7A1st_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7A2nd_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7A2nd_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7A3rd_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7A3rd_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7Alegend_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7Alegend_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7Baci_axis_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7Baci_axis_name</t>
+    <t xml:space="preserve">Fig7A_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7A_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7B_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7B_name</t>
   </si>
   <si>
     <t xml:space="preserve">Fig7C_number</t>
@@ -127,10 +109,28 @@
     <t xml:space="preserve">Fig7C_name</t>
   </si>
   <si>
-    <t xml:space="preserve">Fig7D_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig7D_name</t>
+    <t xml:space="preserve">Fig7ABClegend_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7ABClegend_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7Daci_axis_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7Daci_axis_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7E_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7E_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7F_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fig7F_name</t>
   </si>
   <si>
     <t xml:space="preserve">gray</t>
@@ -151,7 +151,7 @@
     <t xml:space="preserve">wt</t>
   </si>
   <si>
-    <t xml:space="preserve">Aci 110 wt</t>
+    <t xml:space="preserve">Aci 110 (wt)</t>
   </si>
   <si>
     <t xml:space="preserve">Aci 15</t>
@@ -175,7 +175,7 @@
     <t xml:space="preserve">H&lt;sup&gt;R&lt;/sup&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">A110-1 H&lt;sup&gt;R&lt;/sup&gt;</t>
+    <t xml:space="preserve">A110-1 (H&lt;sup&gt;R&lt;/sup&gt;)</t>
   </si>
   <si>
     <t xml:space="preserve">A107-E1</t>
@@ -232,7 +232,7 @@
     <t xml:space="preserve">HS&lt;sup&gt;R&lt;/sup&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">A110-2 HS&lt;sup&gt;R&lt;/sup&gt;</t>
+    <t xml:space="preserve">A110-2 (HS&lt;sup&gt;R&lt;/sup&gt;)</t>
   </si>
   <si>
     <t xml:space="preserve">Aci 110 + HS</t>
@@ -307,7 +307,7 @@
     <t xml:space="preserve">HSFPh&lt;sup&gt;R&lt;/sup&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">A110-G1 HSFPh&lt;sup&gt;R&lt;/sup&gt;</t>
+    <t xml:space="preserve">A110-G1 (HSFPh&lt;sup&gt;R&lt;/sup&gt;)</t>
   </si>
   <si>
     <t xml:space="preserve">Aci 110 + HSFPh</t>
@@ -683,17 +683,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AL14"/>
+  <dimension ref="A1:AL38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="X1" activeCellId="0" sqref="X1"/>
+      <selection pane="topRight" activeCell="AD1" activeCellId="0" sqref="AD1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC14" activeCellId="0" sqref="AC14"/>
+      <selection pane="bottomRight" activeCell="AL2" activeCellId="0" sqref="AL2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.7"/>
@@ -1009,18 +1009,18 @@
       <c r="W3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="X3" s="14" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y3" s="11" t="s">
-        <v>49</v>
-      </c>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="11"/>
       <c r="Z3" s="15"/>
       <c r="AA3" s="11"/>
-      <c r="AB3" s="15"/>
-      <c r="AC3" s="11"/>
+      <c r="AB3" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC3" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="AD3" s="11" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AE3" s="11" t="s">
         <v>51</v>
@@ -1580,18 +1580,18 @@
       <c r="W13" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="11"/>
+      <c r="X13" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y13" s="11" t="s">
+        <v>93</v>
+      </c>
       <c r="Z13" s="15"/>
       <c r="AA13" s="11"/>
-      <c r="AB13" s="15" t="n">
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="11"/>
+      <c r="AD13" s="11" t="n">
         <v>3</v>
-      </c>
-      <c r="AC13" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="AD13" s="11" t="n">
-        <v>5</v>
       </c>
       <c r="AE13" s="11" t="s">
         <v>95</v>
@@ -1668,6 +1668,62 @@
       <c r="AJ14" s="14"/>
       <c r="AK14" s="19"/>
     </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y25" s="0"/>
+      <c r="Z25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y26" s="0"/>
+      <c r="Z26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y27" s="0"/>
+      <c r="Z27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y28" s="0"/>
+      <c r="Z28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y29" s="0"/>
+      <c r="Z29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y30" s="0"/>
+      <c r="Z30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y31" s="0"/>
+      <c r="Z31" s="0"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y32" s="0"/>
+      <c r="Z32" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y33" s="0"/>
+      <c r="Z33" s="0"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y34" s="0"/>
+      <c r="Z34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y35" s="0"/>
+      <c r="Z35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y36" s="0"/>
+      <c r="Z36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y37" s="0"/>
+      <c r="Z37" s="0"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y38" s="0"/>
+      <c r="Z38" s="0"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>